<commit_message>
added DB, need to finish manager methods. DB is populated
</commit_message>
<xml_diff>
--- a/mapPIN - CBL - important data.xlsx
+++ b/mapPIN - CBL - important data.xlsx
@@ -5,18 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/l_batzia_student_tue_nl/Documents/Desktop/Courses/Programming (2IP90)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/r_m_peer_student_tue_nl/Documents/Documents/Coding/Java/CBL_mapPIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{9F791BB6-C3AD-4212-951B-E196D5332EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8926FA71-EE74-4705-BD0B-10C8A559B6CF}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{9F791BB6-C3AD-4212-951B-E196D5332EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCEC40C6-7121-4098-B080-094C04BEE473}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{DA37CB57-3C5C-4177-88C8-FAF6DF0230E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DA37CB57-3C5C-4177-88C8-FAF6DF0230E4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$94</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="286">
   <si>
     <t> Albania</t>
   </si>
@@ -350,6 +354,552 @@
   </si>
   <si>
     <t>creating the map</t>
+  </si>
+  <si>
+    <t>Kabul</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Tirana</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Andorra la Vella</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Yerevan</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Baku</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Manama</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Minsk</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Thimphu</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Sarajevo</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Bandar Seri Begawan</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Zagreb</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Nicosia</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Dili</t>
+  </si>
+  <si>
+    <t>East Timor</t>
+  </si>
+  <si>
+    <t>Tallinn</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Helsinki</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Reykjavik</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Tehran</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Baghdad</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Amman</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Astana</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Pristina</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kuwait City</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Bishkek</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Vientiane</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Riga</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Beirut</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Vaduz</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Vilnius</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg City</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Valletta</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Chisinau</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Ulaanbaatar</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Podgorica</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Naypyidaw</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Pyongyang</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Skopje</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Muscat</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Islamabad</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Warsaw</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Doha</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Bratislava</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Ljubljana</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Jayawardenepura Kotte</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Damascus</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Taipei</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Dushanbe</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Ankara</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Ashgabat</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Kyiv</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>-0.1276</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Tashkent</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vatican City</t>
+  </si>
+  <si>
+    <t>Hanoi</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Sanaa</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Tbilisi</t>
+  </si>
+  <si>
+    <t>Kathmandu</t>
   </si>
 </sst>
 </file>
@@ -387,7 +937,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,1331 +1271,3233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060DF5B0-3575-4B68-B28E-91A26A39C816}">
-  <dimension ref="A1:D94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992AF909-4D4B-4597-8A79-20DFFCD27CF7}">
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="1">
+        <v>345553</v>
+      </c>
+      <c r="D1" s="1">
+        <v>692075</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1">
+        <v>413275</v>
+      </c>
+      <c r="D2" s="1">
+        <v>198189</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="1">
+        <v>425063</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15218</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1">
+        <v>401792</v>
+      </c>
+      <c r="D4" s="1">
+        <v>444991</v>
+      </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1">
+        <v>482082</v>
+      </c>
+      <c r="D5" s="1">
+        <v>163738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="1">
+        <v>404093</v>
+      </c>
+      <c r="D6" s="1">
+        <v>498671</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1">
+        <v>262235</v>
+      </c>
+      <c r="D7" s="1">
+        <v>505876</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="1">
+        <v>238103</v>
+      </c>
+      <c r="D8" s="1">
+        <v>904125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="1">
+        <v>539006</v>
+      </c>
+      <c r="D9" s="1">
+        <v>275590</v>
+      </c>
+      <c r="E9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="1">
+        <v>508503</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43517</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="1">
+        <v>274728</v>
+      </c>
+      <c r="D11" s="1">
+        <v>896390</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="1">
+        <v>438563</v>
+      </c>
+      <c r="D12" s="1">
+        <v>184131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="1">
+        <v>49031</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1149398</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="1">
+        <v>426977</v>
+      </c>
+      <c r="D14" s="1">
+        <v>233219</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="1">
+        <v>115564</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1049282</v>
+      </c>
+      <c r="E15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="1">
+        <v>399042</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1164074</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="1">
+        <v>458150</v>
+      </c>
+      <c r="D17" s="1">
+        <v>159819</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="1">
+        <v>351856</v>
+      </c>
+      <c r="D18" s="1">
+        <v>333823</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="1">
+        <v>500755</v>
+      </c>
+      <c r="D19" s="1">
+        <v>144378</v>
+      </c>
+      <c r="E19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="1">
+        <v>556761</v>
+      </c>
+      <c r="D20" s="1">
+        <v>125683</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-85569</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1255603</v>
+      </c>
+      <c r="E21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="1">
+        <v>594370</v>
+      </c>
+      <c r="D22" s="1">
+        <v>247536</v>
+      </c>
+      <c r="E22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="1">
+        <v>601699</v>
+      </c>
+      <c r="D23" s="1">
+        <v>249384</v>
+      </c>
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="1">
+        <v>488566</v>
+      </c>
+      <c r="D24" s="1">
+        <v>23522</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="1">
+        <v>525200</v>
+      </c>
+      <c r="D25" s="1">
+        <v>134050</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="1">
+        <v>379838</v>
+      </c>
+      <c r="D26" s="1">
+        <v>237275</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="1">
+        <v>223193</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1141694</v>
+      </c>
+      <c r="E27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="1">
+        <v>474979</v>
+      </c>
+      <c r="D28" s="1">
+        <v>190402</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="1">
+        <v>641466</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-219426</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="1">
+        <v>286139</v>
+      </c>
+      <c r="D30" s="1">
+        <v>772090</v>
+      </c>
+      <c r="E30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-62088</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1068456</v>
+      </c>
+      <c r="E31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="1">
+        <v>356892</v>
+      </c>
+      <c r="D32" s="1">
+        <v>513890</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="1">
+        <v>333152</v>
+      </c>
+      <c r="D33" s="1">
+        <v>443661</v>
+      </c>
+      <c r="E33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="1">
+        <v>533498</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-62603</v>
+      </c>
+      <c r="E34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="1">
+        <v>317683</v>
+      </c>
+      <c r="D35" s="1">
+        <v>352137</v>
+      </c>
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="1">
+        <v>419028</v>
+      </c>
+      <c r="D36" s="1">
+        <v>124964</v>
+      </c>
+      <c r="E36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="1">
+        <v>356762</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1396503</v>
+      </c>
+      <c r="E37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="1">
+        <v>319539</v>
+      </c>
+      <c r="D38" s="1">
+        <v>359106</v>
+      </c>
+      <c r="E38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="1">
+        <v>511605</v>
+      </c>
+      <c r="D39" s="1">
+        <v>714704</v>
+      </c>
+      <c r="E39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" s="1">
+        <v>426629</v>
+      </c>
+      <c r="D40" s="1">
+        <v>211655</v>
+      </c>
+      <c r="E40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" s="1">
+        <v>293759</v>
+      </c>
+      <c r="D41" s="1">
+        <v>479774</v>
+      </c>
+      <c r="E41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="1">
+        <v>428746</v>
+      </c>
+      <c r="D42" s="1">
+        <v>745698</v>
+      </c>
+      <c r="E42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" s="1">
+        <v>179757</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1026331</v>
+      </c>
+      <c r="E43" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="1">
+        <v>569496</v>
+      </c>
+      <c r="D44" s="1">
+        <v>241052</v>
+      </c>
+      <c r="E44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>191</v>
+      </c>
+      <c r="C45" s="1">
+        <v>338938</v>
+      </c>
+      <c r="D45" s="1">
+        <v>355018</v>
+      </c>
+      <c r="E45" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="1">
+        <v>471410</v>
+      </c>
+      <c r="D46" s="1">
+        <v>95215</v>
+      </c>
+      <c r="E46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" s="1">
+        <v>546872</v>
+      </c>
+      <c r="D47" s="1">
+        <v>252797</v>
+      </c>
+      <c r="E47" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>197</v>
+      </c>
+      <c r="C48" s="1">
+        <v>496117</v>
+      </c>
+      <c r="D48" s="1">
+        <v>61319</v>
+      </c>
+      <c r="E48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="1">
+        <v>31390</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1016869</v>
+      </c>
+      <c r="E49" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>201</v>
+      </c>
+      <c r="C50" s="1">
+        <v>41755</v>
+      </c>
+      <c r="D50" s="1">
+        <v>735093</v>
+      </c>
+      <c r="E50" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" s="1">
+        <v>358989</v>
+      </c>
+      <c r="D51" s="1">
+        <v>145146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>205</v>
+      </c>
+      <c r="C52" s="1">
+        <v>470105</v>
+      </c>
+      <c r="D52" s="1">
+        <v>288638</v>
+      </c>
+      <c r="E52" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="1">
+        <v>437384</v>
+      </c>
+      <c r="D53" s="1">
+        <v>74246</v>
+      </c>
+      <c r="E53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="1">
+        <v>478864</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1069057</v>
+      </c>
+      <c r="E54" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>55</v>
       </c>
-      <c r="B1">
+      <c r="B55" t="s">
         <v>210</v>
       </c>
+      <c r="C55" s="1">
+        <v>424410</v>
+      </c>
+      <c r="D55" s="1">
+        <v>192627</v>
+      </c>
+      <c r="E55" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" s="1">
+        <v>197633</v>
+      </c>
+      <c r="D56" s="1">
+        <v>960785</v>
+      </c>
+      <c r="E56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>214</v>
+      </c>
+      <c r="C57" s="1">
+        <v>523676</v>
+      </c>
+      <c r="D57" s="1">
+        <v>49041</v>
+      </c>
+      <c r="E57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>216</v>
+      </c>
+      <c r="C58" s="1">
+        <v>390392</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1257625</v>
+      </c>
+      <c r="E58" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>218</v>
+      </c>
+      <c r="C59" s="1">
+        <v>419981</v>
+      </c>
+      <c r="D59" s="1">
+        <v>214254</v>
+      </c>
+      <c r="E59" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="1">
+        <v>599139</v>
+      </c>
+      <c r="D60" s="1">
+        <v>107522</v>
+      </c>
+      <c r="E60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>222</v>
+      </c>
+      <c r="C61" s="1">
+        <v>235859</v>
+      </c>
+      <c r="D61" s="1">
+        <v>584059</v>
+      </c>
+      <c r="E61" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" s="1">
+        <v>336844</v>
+      </c>
+      <c r="D62" s="1">
+        <v>730479</v>
+      </c>
+      <c r="E62" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>226</v>
+      </c>
+      <c r="C63" s="1">
+        <v>145995</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1209842</v>
+      </c>
+      <c r="E63" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>228</v>
+      </c>
+      <c r="C64" s="1">
+        <v>522297</v>
+      </c>
+      <c r="D64" s="1">
+        <v>210122</v>
+      </c>
+      <c r="E64" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>230</v>
+      </c>
+      <c r="C65" s="1">
+        <v>387169</v>
+      </c>
+      <c r="D65" s="1">
+        <v>-91399</v>
+      </c>
+      <c r="E65" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="1">
+        <v>25276987</v>
+      </c>
+      <c r="D66" s="1">
+        <v>51520008</v>
+      </c>
+      <c r="E66" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>234</v>
+      </c>
+      <c r="C67" s="1">
+        <v>444268</v>
+      </c>
+      <c r="D67" s="1">
+        <v>261025</v>
+      </c>
+      <c r="E67" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>236</v>
+      </c>
+      <c r="C68" s="1">
+        <v>557558</v>
+      </c>
+      <c r="D68" s="1">
+        <v>376173</v>
+      </c>
+      <c r="E68" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>238</v>
+      </c>
+      <c r="C69" s="1">
+        <v>439336</v>
+      </c>
+      <c r="D69" s="1">
+        <v>124508</v>
+      </c>
+      <c r="E69" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>239</v>
+      </c>
+      <c r="C70" s="1">
+        <v>247136</v>
+      </c>
+      <c r="D70" s="1">
+        <v>466753</v>
+      </c>
+      <c r="E70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>241</v>
+      </c>
+      <c r="C71" s="1">
+        <v>447866</v>
+      </c>
+      <c r="D71" s="1">
+        <v>204489</v>
+      </c>
+      <c r="E71" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>243</v>
+      </c>
+      <c r="C72" s="1">
+        <v>13521</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1038198</v>
+      </c>
+      <c r="E72" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>244</v>
+      </c>
+      <c r="C73" s="1">
+        <v>481486</v>
+      </c>
+      <c r="D73" s="1">
+        <v>171077</v>
+      </c>
+      <c r="E73" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>246</v>
+      </c>
+      <c r="C74" s="1">
+        <v>460569</v>
+      </c>
+      <c r="D74" s="1">
+        <v>145058</v>
+      </c>
+      <c r="E74" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>248</v>
+      </c>
+      <c r="C75" s="1">
+        <v>375665</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1269780</v>
+      </c>
+      <c r="E75" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="1">
+        <v>404168</v>
+      </c>
+      <c r="D76" s="1">
+        <v>-37038</v>
+      </c>
+      <c r="E76" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77" s="1">
+        <v>69271</v>
+      </c>
+      <c r="D77" s="1">
+        <v>798612</v>
+      </c>
+      <c r="E77" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>254</v>
+      </c>
+      <c r="C78" s="1">
+        <v>593293</v>
+      </c>
+      <c r="D78" s="1">
+        <v>180686</v>
+      </c>
+      <c r="E78" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>256</v>
+      </c>
+      <c r="C79" s="1">
+        <v>469480</v>
+      </c>
+      <c r="D79" s="1">
+        <v>74474</v>
+      </c>
+      <c r="E79" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>258</v>
+      </c>
+      <c r="C80" s="1">
+        <v>335138</v>
+      </c>
+      <c r="D80" s="1">
+        <v>362765</v>
+      </c>
+      <c r="E80" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="1">
+        <v>250330</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1215654</v>
+      </c>
+      <c r="E81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>262</v>
+      </c>
+      <c r="C82" s="1">
+        <v>385598</v>
+      </c>
+      <c r="D82" s="1">
+        <v>687870</v>
+      </c>
+      <c r="E82" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" s="1">
+        <v>137563</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1005018</v>
+      </c>
+      <c r="E83" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>266</v>
+      </c>
+      <c r="C84" s="1">
+        <v>399334</v>
+      </c>
+      <c r="D84" s="1">
+        <v>328597</v>
+      </c>
+      <c r="E84" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>268</v>
+      </c>
+      <c r="C85" s="1">
+        <v>379601</v>
+      </c>
+      <c r="D85" s="1">
+        <v>583261</v>
+      </c>
+      <c r="E85" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>270</v>
+      </c>
+      <c r="C86" s="1">
+        <v>504501</v>
+      </c>
+      <c r="D86" s="1">
+        <v>305234</v>
+      </c>
+      <c r="E86" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>272</v>
+      </c>
+      <c r="C87" s="1">
+        <v>244539</v>
+      </c>
+      <c r="D87" s="1">
+        <v>543773</v>
+      </c>
+      <c r="E87" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>274</v>
+      </c>
+      <c r="C88" s="1">
+        <v>515072</v>
+      </c>
+      <c r="D88" t="s">
+        <v>275</v>
+      </c>
+      <c r="E88" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>277</v>
+      </c>
+      <c r="C89" s="1">
+        <v>412995</v>
+      </c>
+      <c r="D89" s="1">
+        <v>692401</v>
+      </c>
+      <c r="E89" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>279</v>
+      </c>
+      <c r="C90" s="1">
+        <v>419029</v>
+      </c>
+      <c r="D90" s="1">
+        <v>124534</v>
+      </c>
+      <c r="E90" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>280</v>
+      </c>
+      <c r="C91" s="1">
+        <v>210285</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1058542</v>
+      </c>
+      <c r="E91" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>282</v>
+      </c>
+      <c r="C92" s="1">
+        <v>153694</v>
+      </c>
+      <c r="D92" s="1">
+        <v>441910</v>
+      </c>
+      <c r="E92" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>284</v>
+      </c>
+      <c r="C93" s="1">
+        <v>417151</v>
+      </c>
+      <c r="D93" s="1">
+        <v>448271</v>
+      </c>
+      <c r="E93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>285</v>
+      </c>
+      <c r="C94" s="1">
+        <v>277172</v>
+      </c>
+      <c r="D94" s="1">
+        <v>853240</v>
+      </c>
+      <c r="E94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060DF5B0-3575-4B68-B28E-91A26A39C816}">
+  <dimension ref="A1:E94"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
       <c r="C1">
+        <v>210</v>
+      </c>
+      <c r="D1">
         <v>12</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>210</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>210</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>36</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>210</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>48</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5">
         <v>210</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5">
         <v>60</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6">
         <v>160</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6">
         <v>72</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7">
         <v>210</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7">
         <v>84</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>210</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>96</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>210</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>108</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>210</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>120</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>210</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>132</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>210</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>144</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>87</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>210</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>156</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>210</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>168</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>210</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>180</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>210</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>192</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>210</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>204</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
         <v>86</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>210</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>216</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>210</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>228</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20">
         <v>210</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20">
         <v>240</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21">
         <v>160</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21">
         <v>12</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22">
         <v>160</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22">
         <v>36</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23">
         <v>160</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23">
         <v>168</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24">
         <v>160</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24">
         <v>60</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25">
         <v>10</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25">
         <v>108</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26">
         <v>160</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26">
         <v>84</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27">
         <v>160</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27">
         <v>96</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28">
         <v>160</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28">
         <v>108</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29">
         <v>160</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29">
         <v>120</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30">
         <v>160</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30">
         <v>132</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31">
         <v>160</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31">
         <v>144</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32">
         <v>160</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32">
         <v>156</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33">
         <v>160</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33">
         <v>48</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>160</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>180</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>160</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>192</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
         <v>18</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>160</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>204</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>160</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>216</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>160</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>228</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
         <v>48</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>160</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>240</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
         <v>19</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>110</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>12</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>110</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>24</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
         <v>67</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>110</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>36</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
         <v>66</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>110</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>48</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
         <v>20</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>110</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>60</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
         <v>85</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>110</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>72</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
         <v>21</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>110</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>84</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
         <v>22</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>110</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>96</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
         <v>23</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>110</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>108</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>110</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>132</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
         <v>90</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>110</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>144</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
         <v>24</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>110</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>156</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
         <v>25</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>110</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>168</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
         <v>26</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>110</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>180</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
         <v>51</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>110</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>192</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
         <v>27</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>110</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>204</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>110</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>216</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
         <v>28</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>110</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>228</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
         <v>72</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>110</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>240</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
         <v>29</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>60</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>12</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
         <v>30</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>60</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>24</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
         <v>64</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>60</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>36</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
         <v>53</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>60</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>48</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
         <v>65</v>
       </c>
-      <c r="B63">
+      <c r="C63">
         <v>60</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>72</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
         <v>31</v>
       </c>
-      <c r="B64">
+      <c r="C64">
         <v>60</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>84</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
         <v>32</v>
       </c>
-      <c r="B65">
+      <c r="C65">
         <v>60</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>96</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
         <v>84</v>
       </c>
-      <c r="B66">
+      <c r="C66">
         <v>60</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>108</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
         <v>33</v>
       </c>
-      <c r="B67">
+      <c r="C67">
         <v>60</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>120</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
         <v>34</v>
       </c>
-      <c r="B68">
+      <c r="C68">
         <v>60</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>132</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
         <v>35</v>
       </c>
-      <c r="B69">
+      <c r="C69">
         <v>60</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>156</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
         <v>49</v>
       </c>
-      <c r="B70">
+      <c r="C70">
         <v>60</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>168</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
         <v>36</v>
       </c>
-      <c r="B71">
+      <c r="C71">
         <v>60</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>180</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
         <v>89</v>
       </c>
-      <c r="B72">
+      <c r="C72">
         <v>60</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>192</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
         <v>37</v>
       </c>
-      <c r="B73">
+      <c r="C73">
         <v>60</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>204</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
         <v>38</v>
       </c>
-      <c r="B74">
+      <c r="C74">
         <v>60</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>216</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
+      <c r="C75">
         <v>60</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>228</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
         <v>39</v>
       </c>
-      <c r="B76">
+      <c r="C76">
         <v>60</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>240</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
         <v>77</v>
       </c>
-      <c r="B77">
+      <c r="B77" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77">
         <v>10</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>12</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
         <v>40</v>
       </c>
-      <c r="B78">
+      <c r="C78">
         <v>10</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>24</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>210</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
         <v>41</v>
       </c>
-      <c r="B79">
+      <c r="C79">
         <v>10</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <v>36</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>210</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
         <v>68</v>
       </c>
-      <c r="B80">
+      <c r="C80">
         <v>10</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>48</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
+      <c r="C81">
         <v>10</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>60</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>210</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
         <v>71</v>
       </c>
-      <c r="B82">
+      <c r="C82">
         <v>10</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>72</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>210</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
         <v>57</v>
       </c>
-      <c r="B83">
+      <c r="C83">
         <v>10</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>84</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>210</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
         <v>42</v>
       </c>
-      <c r="B84">
+      <c r="C84">
         <v>10</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>96</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
         <v>58</v>
       </c>
-      <c r="B85">
+      <c r="C85">
         <v>10</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>120</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>210</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
         <v>43</v>
       </c>
-      <c r="B86">
+      <c r="C86">
         <v>10</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>132</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
         <v>75</v>
       </c>
-      <c r="B87">
+      <c r="C87">
         <v>10</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <v>144</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
         <v>44</v>
       </c>
-      <c r="B88">
+      <c r="C88">
         <v>10</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <v>156</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
         <v>59</v>
       </c>
-      <c r="B89">
+      <c r="C89">
         <v>10</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <v>168</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
         <v>45</v>
       </c>
-      <c r="B90">
+      <c r="C90">
         <v>10</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>180</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>210</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
         <v>62</v>
       </c>
-      <c r="B91">
+      <c r="C91">
         <v>10</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <v>192</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
         <v>56</v>
       </c>
-      <c r="B92">
+      <c r="C92">
         <v>10</v>
       </c>
-      <c r="C92">
+      <c r="D92">
         <v>204</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
         <v>92</v>
       </c>
-      <c r="B93">
+      <c r="C93">
         <v>10</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>216</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
         <v>93</v>
       </c>
-      <c r="B94">
+      <c r="C94">
         <v>10</v>
       </c>
-      <c r="C94">
+      <c r="D94">
         <v>228</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>210</v>
       </c>
     </row>
@@ -2057,11 +4509,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB448A96-AA9B-43ED-AD18-F65600FB8241}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2121,7 +4573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B96A58-3E40-4A14-B21C-D3F26CCC1E48}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>